<commit_message>
Add the basis logic and basic view
</commit_message>
<xml_diff>
--- a/DevelopSoft/dhl_dotnet_task/dhl_dotnet_task/Customers Data.xlsx
+++ b/DevelopSoft/dhl_dotnet_task/dhl_dotnet_task/Customers Data.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27AA3D13-90C4-4A36-8E08-C36EEDE47942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -2169,7 +2170,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2203,7 +2204,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Нормален" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2480,27 +2481,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2538,7 +2539,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -2576,7 +2577,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -2614,7 +2615,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -2652,7 +2653,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -2690,7 +2691,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -2728,7 +2729,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>55</v>
       </c>
@@ -2766,7 +2767,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>62</v>
       </c>
@@ -2804,7 +2805,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>71</v>
       </c>
@@ -2842,7 +2843,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>79</v>
       </c>
@@ -2880,7 +2881,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>86</v>
       </c>
@@ -2918,7 +2919,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>97</v>
       </c>
@@ -2956,7 +2957,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>103</v>
       </c>
@@ -2994,7 +2995,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>112</v>
       </c>
@@ -3032,7 +3033,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>118</v>
       </c>
@@ -3070,7 +3071,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>125</v>
       </c>
@@ -3108,7 +3109,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>135</v>
       </c>
@@ -3146,7 +3147,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>142</v>
       </c>
@@ -3184,7 +3185,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>148</v>
       </c>
@@ -3222,7 +3223,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>155</v>
       </c>
@@ -3260,7 +3261,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>162</v>
       </c>
@@ -3298,7 +3299,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>169</v>
       </c>
@@ -3336,7 +3337,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>178</v>
       </c>
@@ -3374,7 +3375,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>189</v>
       </c>
@@ -3412,7 +3413,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>196</v>
       </c>
@@ -3450,7 +3451,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>202</v>
       </c>
@@ -3488,7 +3489,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>210</v>
       </c>
@@ -3526,7 +3527,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>217</v>
       </c>
@@ -3564,7 +3565,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>224</v>
       </c>
@@ -3602,7 +3603,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>230</v>
       </c>
@@ -3640,7 +3641,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>238</v>
       </c>
@@ -3678,7 +3679,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>246</v>
       </c>
@@ -3716,7 +3717,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>253</v>
       </c>
@@ -3754,7 +3755,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>259</v>
       </c>
@@ -3792,7 +3793,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>266</v>
       </c>
@@ -3830,7 +3831,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>274</v>
       </c>
@@ -3868,7 +3869,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>283</v>
       </c>
@@ -3906,7 +3907,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>292</v>
       </c>
@@ -3944,7 +3945,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>300</v>
       </c>
@@ -3982,7 +3983,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>307</v>
       </c>
@@ -4020,7 +4021,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>316</v>
       </c>
@@ -4058,7 +4059,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>324</v>
       </c>
@@ -4096,7 +4097,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>330</v>
       </c>
@@ -4134,7 +4135,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>337</v>
       </c>
@@ -4172,7 +4173,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>344</v>
       </c>
@@ -4210,7 +4211,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>352</v>
       </c>
@@ -4248,7 +4249,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>360</v>
       </c>
@@ -4286,7 +4287,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>367</v>
       </c>
@@ -4324,7 +4325,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>374</v>
       </c>
@@ -4362,7 +4363,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>382</v>
       </c>
@@ -4400,7 +4401,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>390</v>
       </c>
@@ -4438,7 +4439,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>397</v>
       </c>
@@ -4476,7 +4477,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>404</v>
       </c>
@@ -4514,7 +4515,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>413</v>
       </c>
@@ -4552,7 +4553,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>422</v>
       </c>
@@ -4590,7 +4591,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>428</v>
       </c>
@@ -4628,7 +4629,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>435</v>
       </c>
@@ -4666,7 +4667,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>441</v>
       </c>
@@ -4704,7 +4705,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>449</v>
       </c>
@@ -4742,7 +4743,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>456</v>
       </c>
@@ -4780,7 +4781,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>463</v>
       </c>
@@ -4818,7 +4819,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>469</v>
       </c>
@@ -4856,7 +4857,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>476</v>
       </c>
@@ -4894,7 +4895,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>481</v>
       </c>
@@ -4932,7 +4933,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>482</v>
       </c>
@@ -4970,7 +4971,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>489</v>
       </c>
@@ -5008,7 +5009,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>495</v>
       </c>
@@ -5046,7 +5047,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>501</v>
       </c>
@@ -5084,7 +5085,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>507</v>
       </c>
@@ -5122,7 +5123,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>516</v>
       </c>
@@ -5160,7 +5161,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>523</v>
       </c>
@@ -5198,7 +5199,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>529</v>
       </c>
@@ -5236,7 +5237,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>535</v>
       </c>
@@ -5274,7 +5275,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>541</v>
       </c>
@@ -5312,7 +5313,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>549</v>
       </c>
@@ -5350,7 +5351,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>556</v>
       </c>
@@ -5388,7 +5389,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>563</v>
       </c>
@@ -5426,7 +5427,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>571</v>
       </c>
@@ -5464,7 +5465,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>577</v>
       </c>
@@ -5502,7 +5503,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>585</v>
       </c>
@@ -5540,7 +5541,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>593</v>
       </c>
@@ -5578,7 +5579,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>598</v>
       </c>
@@ -5616,7 +5617,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>606</v>
       </c>
@@ -5654,7 +5655,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>613</v>
       </c>
@@ -5692,7 +5693,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>618</v>
       </c>
@@ -5730,7 +5731,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>625</v>
       </c>
@@ -5768,7 +5769,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>632</v>
       </c>
@@ -5806,7 +5807,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>639</v>
       </c>
@@ -5844,7 +5845,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>646</v>
       </c>
@@ -5882,7 +5883,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>653</v>
       </c>
@@ -5920,7 +5921,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>660</v>
       </c>
@@ -5958,7 +5959,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>667</v>
       </c>
@@ -5996,7 +5997,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>674</v>
       </c>
@@ -6034,7 +6035,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>681</v>
       </c>
@@ -6072,7 +6073,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>688</v>
       </c>
@@ -6110,7 +6111,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>695</v>
       </c>
@@ -6148,7 +6149,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>703</v>
       </c>
@@ -6186,7 +6187,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>710</v>
       </c>
@@ -6224,7 +6225,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>712</v>
       </c>

</xml_diff>